<commit_message>
cleanup and reannotate PCB
</commit_message>
<xml_diff>
--- a/Motherboard/REV20200407C/reviews/PCB.xlsx
+++ b/Motherboard/REV20200407C/reviews/PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\git\SensorCard\Motherboard\REV20200407C\reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25678D45-2110-4412-A067-F425F4E22978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D5570-EDC3-4750-800F-23CCDDB87794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12330" yWindow="-14510" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group_18May" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Reviews</t>
   </si>
@@ -109,14 +109,38 @@
     <t>Square first pin marker for throu hole</t>
   </si>
   <si>
-    <t>Required one mounting hole near AMDC connector</t>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Hommond mounting rack</t>
+  </si>
+  <si>
+    <t>The horizontal seperation of most of the mounting holes match with the pitch of this -&gt;</t>
+  </si>
+  <si>
+    <t>Required one extra mounting hole near the right side (close to connectors)</t>
+  </si>
+  <si>
+    <t>The shew is 6.5% in the longest trace.</t>
+  </si>
+  <si>
+    <t>GND plane in  bottom removed. I have tented all other vias</t>
+  </si>
+  <si>
+    <t>Please let me know if this fine</t>
+  </si>
+  <si>
+    <t>Because of lack of space, moved existing center mounting hole to the right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +152,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,10 +197,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -178,8 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,36 +495,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92E892-9BD6-433E-A9BE-9B443AC07D54}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="72.90625" customWidth="1"/>
     <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -498,62 +536,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -569,43 +626,46 @@
       <c r="C18" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{8C7B378B-4B63-42A7-B02C-58632004BFDB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="72.90625" customWidth="1"/>
     <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -616,14 +676,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -632,7 +699,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -643,7 +710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -652,7 +719,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -661,7 +728,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -670,7 +737,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -679,7 +746,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -688,7 +755,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -697,7 +764,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>